<commit_message>
Empesando Agregar grado y colegio
</commit_message>
<xml_diff>
--- a/ayudas/diseño relacion polimorfica de uno a uno.xlsx
+++ b/ayudas/diseño relacion polimorfica de uno a uno.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>id</t>
   </si>
@@ -111,13 +112,124 @@
   </si>
   <si>
     <t>Inscripcion</t>
+  </si>
+  <si>
+    <t>estudiante</t>
+  </si>
+  <si>
+    <t>estudiante1</t>
+  </si>
+  <si>
+    <t>estudiante2</t>
+  </si>
+  <si>
+    <t>estudiante3</t>
+  </si>
+  <si>
+    <t>estudiante4</t>
+  </si>
+  <si>
+    <t>estudiante5</t>
+  </si>
+  <si>
+    <t>estudiante6</t>
+  </si>
+  <si>
+    <t>estudiante7</t>
+  </si>
+  <si>
+    <t>estudiante8</t>
+  </si>
+  <si>
+    <t>estudiante9</t>
+  </si>
+  <si>
+    <t>estudiante10</t>
+  </si>
+  <si>
+    <t>estudiante11</t>
+  </si>
+  <si>
+    <t>estudiante12</t>
+  </si>
+  <si>
+    <t>estudiante13</t>
+  </si>
+  <si>
+    <t>estudiante14</t>
+  </si>
+  <si>
+    <t>estudiante_grado_colegio</t>
+  </si>
+  <si>
+    <t>colegio</t>
+  </si>
+  <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t>col2</t>
+  </si>
+  <si>
+    <t>col3</t>
+  </si>
+  <si>
+    <t>col4</t>
+  </si>
+  <si>
+    <t>col5</t>
+  </si>
+  <si>
+    <t>col6</t>
+  </si>
+  <si>
+    <t>col7</t>
+  </si>
+  <si>
+    <t>col8</t>
+  </si>
+  <si>
+    <t>col9</t>
+  </si>
+  <si>
+    <t>col10</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>grado1</t>
+  </si>
+  <si>
+    <t>grado2</t>
+  </si>
+  <si>
+    <t>grado3</t>
+  </si>
+  <si>
+    <t>grado4</t>
+  </si>
+  <si>
+    <t>grado5</t>
+  </si>
+  <si>
+    <t>grado6</t>
+  </si>
+  <si>
+    <t>grado7</t>
+  </si>
+  <si>
+    <t>grado8</t>
+  </si>
+  <si>
+    <t>grado9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,16 +237,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,16 +282,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -460,277 +648,277 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="F15" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="F15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>2</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
         <v>2</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>4</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
         <v>3</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>5</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2"/>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>6</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>3</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>5</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>6</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -742,4 +930,702 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="3"/>
+    <col min="6" max="6" width="4.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="3" customWidth="1"/>
+    <col min="9" max="11" width="11.42578125" style="3"/>
+    <col min="12" max="14" width="5.7109375" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
+        <v>2</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
+        <v>3</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
+        <v>4</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <v>5</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2001</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
+        <v>6</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2002</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4">
+        <v>7</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2003</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4">
+        <v>8</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2003</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4">
+        <v>9</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4">
+        <v>10</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4">
+        <v>13</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4">
+        <v>1</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4">
+        <v>2</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4">
+        <v>3</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4">
+        <v>4</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4">
+        <v>5</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4">
+        <v>6</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4">
+        <v>7</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="4">
+        <v>8</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="4">
+        <v>9</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L6:N6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ya estamos a punto de mostrar los grados y colegios
</commit_message>
<xml_diff>
--- a/ayudas/diseño relacion polimorfica de uno a uno.xlsx
+++ b/ayudas/diseño relacion polimorfica de uno a uno.xlsx
@@ -254,7 +254,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,8 +344,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -937,98 +937,98 @@
   <dimension ref="A2:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="6" width="4.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="3" customWidth="1"/>
-    <col min="9" max="11" width="11.42578125" style="3"/>
-    <col min="12" max="14" width="5.7109375" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="2" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="4"/>
+    <col min="6" max="6" width="4.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="4" customWidth="1"/>
+    <col min="9" max="11" width="11.42578125" style="4"/>
+    <col min="12" max="14" width="5.7109375" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="5" t="s">
         <v>45</v>
       </c>
@@ -1036,588 +1036,588 @@
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4">
-        <v>1</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
         <v>2</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
         <v>3</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
         <v>4</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
         <v>2000</v>
       </c>
-      <c r="I11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4">
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3">
         <v>5</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
         <v>2</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>2001</v>
       </c>
-      <c r="I12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4">
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3">
         <v>6</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
         <v>2</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>2002</v>
       </c>
-      <c r="I13" s="4">
-        <v>1</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4">
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3">
         <v>7</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
         <v>3</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>2003</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>2</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
         <v>8</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
         <v>3</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>2003</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>3</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3">
         <v>9</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="4"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3">
         <v>6</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3">
         <v>10</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3">
         <v>7</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
         <v>8</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3">
         <v>9</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3">
         <v>10</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3">
         <v>11</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3">
         <v>12</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
         <v>13</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3">
         <v>14</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4">
-        <v>1</v>
-      </c>
-      <c r="K25" s="4" t="s">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3">
+        <v>1</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3">
         <v>2</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3">
         <v>3</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3">
         <v>4</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3">
         <v>5</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3">
         <v>6</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3">
         <v>7</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J32" s="4">
+      <c r="J32" s="3">
         <v>8</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J33" s="4">
+      <c r="J33" s="3">
         <v>9</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambiado la relacion de userable se elimino el model Userable
</commit_message>
<xml_diff>
--- a/ayudas/diseño relacion polimorfica de uno a uno.xlsx
+++ b/ayudas/diseño relacion polimorfica de uno a uno.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <t>id</t>
   </si>
@@ -239,12 +240,84 @@
   </si>
   <si>
     <t>calificable_type</t>
+  </si>
+  <si>
+    <t>MATRICULACIONS</t>
+  </si>
+  <si>
+    <t>FDSFDS</t>
+  </si>
+  <si>
+    <t>FDS</t>
+  </si>
+  <si>
+    <t>GFDG</t>
+  </si>
+  <si>
+    <t>GFDGGF</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>GH</t>
+  </si>
+  <si>
+    <t>HGH</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>OBSERVACIONS</t>
+  </si>
+  <si>
+    <t>OBSER</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>OBSERVABLE_ID</t>
+  </si>
+  <si>
+    <t>OBSERVABLE_TYPE</t>
+  </si>
+  <si>
+    <t>observacion 1</t>
+  </si>
+  <si>
+    <t>observacion 2</t>
+  </si>
+  <si>
+    <t>observacion 3</t>
+  </si>
+  <si>
+    <t>observacion 4</t>
+  </si>
+  <si>
+    <t>observacion 5</t>
+  </si>
+  <si>
+    <t>observacion 6</t>
+  </si>
+  <si>
+    <t>observacion 7</t>
+  </si>
+  <si>
+    <t>matr</t>
+  </si>
+  <si>
+    <t>insc</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,12 +464,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,13 +490,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -697,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H33"/>
+  <dimension ref="B5:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,13 +785,13 @@
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -731,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>2</v>
       </c>
@@ -739,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>3</v>
       </c>
@@ -747,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>4</v>
       </c>
@@ -755,7 +831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>5</v>
       </c>
@@ -763,7 +839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>6</v>
       </c>
@@ -771,14 +847,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="8" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="K14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -793,7 +872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,10 +1076,186 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,17 +1327,17 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="7"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>69</v>
@@ -1218,10 +1473,10 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="7"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1293,11 +1548,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -1390,11 +1645,11 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="7"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
falta cambiar estado de la inscripcion y matriculacion finalizada
</commit_message>
<xml_diff>
--- a/ayudas/diseño relacion polimorfica de uno a uno.xlsx
+++ b/ayudas/diseño relacion polimorfica de uno a uno.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -312,6 +313,21 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>mensajeable_id</t>
+  </si>
+  <si>
+    <t>mensajeable_type</t>
+  </si>
+  <si>
+    <t>mensaje_id</t>
+  </si>
+  <si>
+    <t>persona_id</t>
+  </si>
+  <si>
+    <t>inscripcion</t>
   </si>
 </sst>
 </file>
@@ -464,11 +480,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +500,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,9 +510,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -775,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,10 +805,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -848,20 +867,20 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
       <c r="K14" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="F15" s="1" t="s">
         <v>24</v>
       </c>
@@ -999,10 +1018,10 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="5"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1091,11 +1110,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
       <c r="I5" t="s">
         <v>80</v>
       </c>
@@ -1178,11 +1197,11 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="G10">
         <v>4</v>
       </c>
@@ -1254,7 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1265,10 +1284,10 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1327,17 +1346,17 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="8"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>69</v>
@@ -1473,10 +1492,10 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="8"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1552,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -1645,11 +1664,11 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -2244,4 +2263,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C10:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>